<commit_message>
Created two new forms for registering new players and teams and created a batch players upload option usign excel or csv files(Beta)
</commit_message>
<xml_diff>
--- a/jpl sample data.xlsx
+++ b/jpl sample data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\JPL\jpl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\JPL 2\JPL-frontend\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>name</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Prathamesh Bhadwalkar</t>
+  </si>
+  <si>
+    <t>base_price</t>
   </si>
 </sst>
 </file>
@@ -406,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,9 +421,10 @@
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -433,8 +437,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
@@ -447,8 +454,11 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="E2">
+        <v>25000</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -461,8 +471,11 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E3">
+        <v>25000</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -475,8 +488,11 @@
       <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E4">
+        <v>25000</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -489,8 +505,11 @@
       <c r="D5" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E5">
+        <v>25000</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -502,6 +521,9 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>15</v>
+      </c>
+      <c r="E6">
+        <v>25000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>